<commit_message>
added tags for script
</commit_message>
<xml_diff>
--- a/Documentation/Journal&Plan/JournalDeTravail-ShansheGundishvili.xlsx
+++ b/Documentation/Journal&Plan/JournalDeTravail-ShansheGundishvili.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PHPModel\Documentation\Journal&amp;Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9C0882-CA9E-4B22-B00A-E4A24ABD354D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167FABEA-9715-4A4B-AB55-B456670E577F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>Jour</t>
   </si>
@@ -175,6 +175,30 @@
   </si>
   <si>
     <t>Fixing de template en general</t>
+  </si>
+  <si>
+    <t>newsletter fini</t>
+  </si>
+  <si>
+    <t>contact fini</t>
+  </si>
+  <si>
+    <t>Gallery frontend fini</t>
+  </si>
+  <si>
+    <t>Gallery backend fini</t>
+  </si>
+  <si>
+    <t>Gallery modify fini</t>
+  </si>
+  <si>
+    <t>documentation general</t>
+  </si>
+  <si>
+    <t>Il n'y avait pas de diagramme avec les exigences que je voulais utiliser, j'ai donc utilisé UML mais cela ne correspond pas aux normes.</t>
+  </si>
+  <si>
+    <t>Structure de code de site</t>
   </si>
 </sst>
 </file>
@@ -296,10 +320,10 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,10 +641,10 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="13"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
@@ -646,8 +670,8 @@
         <v>10</v>
       </c>
       <c r="I2" s="11">
-        <f>SUM(C2:C21)</f>
-        <v>53.75</v>
+        <f>SUM(C2:C26)</f>
+        <v>67.75</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -670,7 +694,7 @@
       <c r="F3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1043,13 +1067,160 @@
         <v>3.25</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>45068</v>
+      </c>
+      <c r="B22" s="6">
+        <f t="shared" ref="B22" si="12">WEEKNUM(A22)</f>
+        <v>21</v>
+      </c>
+      <c r="C22" s="8">
+        <v>3.25</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>45068</v>
+      </c>
+      <c r="B23" s="6">
+        <f t="shared" ref="B23:B24" si="13">WEEKNUM(A23)</f>
+        <v>21</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>45069</v>
+      </c>
+      <c r="B24" s="6">
+        <f t="shared" si="13"/>
+        <v>21</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2.25</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>45069</v>
+      </c>
+      <c r="B25" s="6">
+        <f t="shared" ref="B25" si="14">WEEKNUM(A25)</f>
+        <v>21</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>45069</v>
+      </c>
+      <c r="B26" s="6">
+        <f t="shared" ref="B26" si="15">WEEKNUM(A26)</f>
+        <v>21</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>45071</v>
+      </c>
+      <c r="B27" s="6">
+        <f t="shared" ref="B27:B28" si="16">WEEKNUM(A27)</f>
+        <v>21</v>
+      </c>
+      <c r="C27" s="8">
+        <v>5.25</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>45072</v>
+      </c>
+      <c r="B28" s="6">
+        <f t="shared" si="16"/>
+        <v>21</v>
+      </c>
+      <c r="C28" s="8">
+        <v>5.25</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed  tags for script
</commit_message>
<xml_diff>
--- a/Documentation/Journal&Plan/JournalDeTravail-ShansheGundishvili.xlsx
+++ b/Documentation/Journal&Plan/JournalDeTravail-ShansheGundishvili.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PHPModel\Documentation\Journal&amp;Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167FABEA-9715-4A4B-AB55-B456670E577F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D4EA90-AB66-422F-A025-A792169C4EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>Jour</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Structure de code de site</t>
+  </si>
+  <si>
+    <t>documentation de toutes les fonctions</t>
+  </si>
+  <si>
+    <t>tagging the code for the script</t>
   </si>
 </sst>
 </file>
@@ -604,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,8 +676,8 @@
         <v>10</v>
       </c>
       <c r="I2" s="11">
-        <f>SUM(C2:C26)</f>
-        <v>67.75</v>
+        <f>SUM(C2:C30)</f>
+        <v>83.5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1221,6 +1227,48 @@
       </c>
       <c r="F28" s="9" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>45076</v>
+      </c>
+      <c r="B29" s="6">
+        <f t="shared" ref="B29" si="17">WEEKNUM(A29)</f>
+        <v>22</v>
+      </c>
+      <c r="C29" s="8">
+        <v>2</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>45076</v>
+      </c>
+      <c r="B30" s="6">
+        <f t="shared" ref="B30" si="18">WEEKNUM(A30)</f>
+        <v>22</v>
+      </c>
+      <c r="C30" s="8">
+        <v>3.25</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>